<commit_message>
manually update al files to old reference style
</commit_message>
<xml_diff>
--- a/data/TranslationFileUTF8.xlsx
+++ b/data/TranslationFileUTF8.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WS\PACTA\PACTA_analysis\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clare\Dropbox (2° Investing)\2° Investing Team\People\clare\GitHub\Reference\ReferenceData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933E3F06-D306-47CC-994F-2889585FE59D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="16770" windowWidth="28790" windowHeight="15590"/>
+    <workbookView xWindow="15" yWindow="16770" windowWidth="28785" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TranslationFileUTF8" sheetId="1" r:id="rId1"/>
@@ -17,10 +18,10 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TranslationFileUTF8!$A$1:$E$299</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="330"/>
+      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1525" uniqueCount="1343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1525" uniqueCount="1342">
   <si>
     <t>TextLabel</t>
   </si>
@@ -4059,15 +4060,12 @@
   </si>
   <si>
     <t>Compatible1.5</t>
-  </si>
-  <si>
-    <t>YourPortfoliohasnoproductioninthissectorfortheselectedscenario_geographyandMarket</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -4708,133 +4706,133 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="126"/>
   </cellXfs>
   <cellStyles count="127">
-    <cellStyle name="20 % - Dekorfärg1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Dekorfärg2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Dekorfärg3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Dekorfärg4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Dekorfärg5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Dekorfärg6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Dekorfärg1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Dekorfärg2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Dekorfärg3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Dekorfärg4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Dekorfärg5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Dekorfärg6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Dekorfärg1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Dekorfärg2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Dekorfärg3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Dekorfärg4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Dekorfärg5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Dekorfärg6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Anteckning" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Beräkning" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Bra" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Dålig" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Dekorfärg1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Dekorfärg2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Dekorfärg3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Dekorfärg4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Dekorfärg5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Dekorfärg6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="45" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="47" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="49" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="51" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="53" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="55" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="57" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="59" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="61" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="63" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="65" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="67" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="69" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="71" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="73" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="75" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="77" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="79" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="81" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="83" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="85" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="87" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="89" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="91" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="93" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="95" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="97" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="99" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="101" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="103" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="105" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="107" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="109" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="111" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="113" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="115" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="117" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="119" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="121" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="123" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="125" builtinId="9" hidden="1"/>
-    <cellStyle name="Förklarande text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Hyperlänk" xfId="42" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="44" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="46" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="48" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="50" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="52" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="54" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="56" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="58" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="60" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="62" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="64" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="66" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="68" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="70" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="72" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="74" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="76" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="78" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="80" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="82" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="84" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="86" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="88" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="90" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="92" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="94" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="96" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="98" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="100" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="102" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="104" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="106" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="108" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="110" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="112" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="114" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="116" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="118" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="120" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="122" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="124" builtinId="8" hidden="1"/>
-    <cellStyle name="Indata" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Kontrollcell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Länkad cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="126"/>
-    <cellStyle name="Rubrik" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Rubrik 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Rubrik 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Rubrik 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Rubrik 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Summa" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Utdata" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Varningstext" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Normal 2" xfId="126" xr:uid="{D933FAF0-4B79-49EC-896B-EDD28F872E5D}"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5145,11 +5143,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E325"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" zoomScale="80" zoomScaleNormal="247" workbookViewId="0">
-      <selection activeCell="A197" sqref="A197"/>
+    <sheetView tabSelected="1" topLeftCell="A310" zoomScale="80" zoomScaleNormal="247" workbookViewId="0">
+      <selection activeCell="A320" sqref="A320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -8411,7 +8409,7 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>1342</v>
+        <v>551</v>
       </c>
       <c r="B197" t="s">
         <v>713</v>
@@ -10390,7 +10388,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E299"/>
+  <autoFilter ref="A1:E299" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
revert changes to data/
</commit_message>
<xml_diff>
--- a/data/TranslationFileUTF8.xlsx
+++ b/data/TranslationFileUTF8.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clare\Dropbox (2° Investing)\2° Investing Team\People\clare\GitHub\Reference\ReferenceData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WS\PACTA\PACTA_analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933E3F06-D306-47CC-994F-2889585FE59D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="16770" windowWidth="28785" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="16770" windowWidth="28790" windowHeight="15590"/>
   </bookViews>
   <sheets>
     <sheet name="TranslationFileUTF8" sheetId="1" r:id="rId1"/>
@@ -18,10 +17,10 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TranslationFileUTF8!$A$1:$E$299</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1525" uniqueCount="1342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1525" uniqueCount="1343">
   <si>
     <t>TextLabel</t>
   </si>
@@ -4060,12 +4059,15 @@
   </si>
   <si>
     <t>Compatible1.5</t>
+  </si>
+  <si>
+    <t>YourPortfoliohasnoproductioninthissectorfortheselectedscenario_geographyandMarket</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -4706,133 +4708,133 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="126"/>
   </cellXfs>
   <cellStyles count="127">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20 % - Dekorfärg1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Dekorfärg2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Dekorfärg3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Dekorfärg4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Dekorfärg5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Dekorfärg6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Dekorfärg1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Dekorfärg2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Dekorfärg3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Dekorfärg4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Dekorfärg5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Dekorfärg6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Dekorfärg1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Dekorfärg2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Dekorfärg3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Dekorfärg4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Dekorfärg5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Dekorfärg6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Anteckning" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Beräkning" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Bra" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Dålig" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Dekorfärg1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Dekorfärg2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Dekorfärg3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Dekorfärg4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Dekorfärg5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Dekorfärg6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Förklarande text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Hyperlänk" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Indata" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Kontrollcell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Länkad cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="126" xr:uid="{D933FAF0-4B79-49EC-896B-EDD28F872E5D}"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Normal 2" xfId="126"/>
+    <cellStyle name="Rubrik" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Rubrik 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Rubrik 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Rubrik 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Rubrik 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Summa" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Utdata" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Varningstext" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5143,11 +5145,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E325"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A310" zoomScale="80" zoomScaleNormal="247" workbookViewId="0">
-      <selection activeCell="A320" sqref="A320"/>
+    <sheetView tabSelected="1" topLeftCell="A185" zoomScale="80" zoomScaleNormal="247" workbookViewId="0">
+      <selection activeCell="A197" sqref="A197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -8409,7 +8411,7 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>551</v>
+        <v>1342</v>
       </c>
       <c r="B197" t="s">
         <v>713</v>
@@ -10388,7 +10390,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E299" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E299"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>